<commit_message>
added more data in the test plan
</commit_message>
<xml_diff>
--- a/Test Plan.xlsx
+++ b/Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68336143c0100ff2/Desktop/All_Files/Software Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{D8FAA641-336C-4084-A9E9-A0FF02FC7DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA3DFAA6-4258-42F2-93DF-8E0A06046F6B}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{D8FAA641-336C-4084-A9E9-A0FF02FC7DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EDF5F8A-E0EE-47CD-8728-4BD77367EF2B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{31341FFD-30FD-4340-A6EB-558596D55CE2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -91,6 +91,24 @@
   </si>
   <si>
     <t>Manual Testing,Bug testing via Excel</t>
+  </si>
+  <si>
+    <t>Test Deliverables</t>
+  </si>
+  <si>
+    <t>Test Cases Documents,bug Report,Final Summary</t>
+  </si>
+  <si>
+    <t>Testing Tools</t>
+  </si>
+  <si>
+    <t>Browser dev tools,Postman,Excel</t>
+  </si>
+  <si>
+    <t>Environments Requeriments</t>
+  </si>
+  <si>
+    <t>Crome,MongoDB,Spring Boot</t>
   </si>
 </sst>
 </file>
@@ -146,6 +164,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -445,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F92317-7933-4730-A4A4-41333DBFBAB4}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,6 +580,39 @@
         <v>18</v>
       </c>
     </row>
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
complet the test plan of the money mate project
</commit_message>
<xml_diff>
--- a/Test Plan.xlsx
+++ b/Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68336143c0100ff2/Desktop/All_Files/Software Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{D8FAA641-336C-4084-A9E9-A0FF02FC7DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EDF5F8A-E0EE-47CD-8728-4BD77367EF2B}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{D8FAA641-336C-4084-A9E9-A0FF02FC7DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABDF8DDE-8662-47C3-9874-975B8EC89EE1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{31341FFD-30FD-4340-A6EB-558596D55CE2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Sr.No.</t>
   </si>
@@ -109,6 +109,42 @@
   </si>
   <si>
     <t>Crome,MongoDB,Spring Boot</t>
+  </si>
+  <si>
+    <t>Role and Responsibilities</t>
+  </si>
+  <si>
+    <t>Govind: UI; Partner: Backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Schedule</t>
+  </si>
+  <si>
+    <t>Writing: 7 Apr, Execution: 8–9 Apr, Bug Fixing: 10 Apr, Final: 11 Apr</t>
+  </si>
+  <si>
+    <t>Risks and Mitigation</t>
+  </si>
+  <si>
+    <t>Internet issue → offline tools, Backend delay → mock data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Entry Criteria</t>
+  </si>
+  <si>
+    <t>Local deployment, Working modules</t>
+  </si>
+  <si>
+    <t>Exit Criteria</t>
+  </si>
+  <si>
+    <t>Major bugs fixed, All test cases passed</t>
+  </si>
+  <si>
+    <t>Approval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	(Leave blank or write “Faculty signature here”)</t>
   </si>
 </sst>
 </file>
@@ -467,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F92317-7933-4730-A4A4-41333DBFBAB4}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,6 +649,72 @@
         <v>24</v>
       </c>
     </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>